<commit_message>
plotted tauc bedload thresholds
</commit_message>
<xml_diff>
--- a/Shear Stress/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/Shear Stress/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Shear Stress\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F99E5B-3D99-4D4F-B981-61EF4377EBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3154BAE-56F2-4399-9988-967DA65F1760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
@@ -173,10 +173,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -340,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,6 +445,15 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,16 +469,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7408,18 +7413,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="39"/>
       <c r="H2" s="18" t="s">
         <v>16</v>
       </c>
@@ -7718,12 +7723,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="24">
@@ -8158,10 +8163,10 @@
       <c r="F1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="39"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8190,11 +8195,11 @@
         <f>$I$20+($I$19-$I$20)*EXP(-14*A2)</f>
         <v>1.3290468742698638</v>
       </c>
-      <c r="H2" s="39" t="str">
+      <c r="H2" s="42" t="str">
         <f>B1</f>
         <v>Tri* (Dg/Ds = 10)</v>
       </c>
-      <c r="I2" s="39"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8322,11 +8327,11 @@
         <f t="shared" si="4"/>
         <v>0.7870350317127095</v>
       </c>
-      <c r="H6" s="39" t="str">
+      <c r="H6" s="42" t="str">
         <f>C1</f>
         <v>Tri* (Dg/Ds = 20)</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8454,11 +8459,11 @@
         <f t="shared" si="4"/>
         <v>0.4774329545306662</v>
       </c>
-      <c r="H10" s="39" t="str">
+      <c r="H10" s="42" t="str">
         <f>D1</f>
         <v>Tri* (Dg/Ds = 35)</v>
       </c>
-      <c r="I10" s="39"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -8586,11 +8591,11 @@
         <f t="shared" si="4"/>
         <v>0.30058544185786273</v>
       </c>
-      <c r="H14" s="39" t="str">
+      <c r="H14" s="42" t="str">
         <f>E1</f>
         <v>Tri* (Dg/Ds = 50)</v>
       </c>
-      <c r="I14" s="39"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -8715,11 +8720,11 @@
         <f t="shared" si="4"/>
         <v>0.1995685397000391</v>
       </c>
-      <c r="H18" s="39" t="str">
+      <c r="H18" s="42" t="str">
         <f>F1</f>
         <v>Tri* (Dg/Ds = 43.4)</v>
       </c>
-      <c r="I18" s="39"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -9238,7 +9243,7 @@
       <c r="M35" s="6">
         <v>0.96462000000000003</v>
       </c>
-      <c r="N35" s="40">
+      <c r="N35" s="35">
         <v>0.86746324999999902</v>
       </c>
     </row>
@@ -11000,7 +11005,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11023,13 +11028,13 @@
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -11062,140 +11067,140 @@
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="36">
         <v>0.21715999999999999</v>
       </c>
       <c r="C3" s="10">
         <f>$B3*($B$11-$B$10)*$B$12*(C$2/1000)</f>
-        <v>1.3235539288509997</v>
+        <v>1.7569299940499998</v>
       </c>
       <c r="D3" s="10">
         <f t="shared" ref="D3:G3" si="0">$B3*($B$11-$B$10)*$B$12*(D$2/1000)</f>
-        <v>1.9853308932764995</v>
+        <v>2.6353949910749996</v>
       </c>
       <c r="E3" s="10">
         <f t="shared" si="0"/>
-        <v>2.6471078577019993</v>
+        <v>3.5138599880999997</v>
       </c>
       <c r="F3" s="10">
         <f t="shared" si="0"/>
-        <v>3.970661786552999</v>
+        <v>5.2707899821499993</v>
       </c>
       <c r="G3" s="10">
         <f t="shared" si="0"/>
-        <v>5.2942157154039986</v>
+        <v>7.0277199761999993</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="45">
         <v>0.40402499999999902</v>
       </c>
       <c r="C4" s="10">
-        <f t="shared" ref="C4:G7" si="1">$B4*($B$11-$B$10)*$B$12*(C$2/1000)</f>
-        <v>2.4624648927243689</v>
+        <f t="shared" ref="C4:G6" si="1">$B4*($B$11-$B$10)*$B$12*(C$2/1000)</f>
+        <v>3.2687587071562421</v>
       </c>
       <c r="D4" s="10">
         <f t="shared" si="1"/>
-        <v>3.6936973390865533</v>
+        <v>4.9031380607343635</v>
       </c>
       <c r="E4" s="10">
         <f t="shared" si="1"/>
-        <v>4.9249297854487377</v>
+        <v>6.5375174143124841</v>
       </c>
       <c r="F4" s="10">
         <f t="shared" si="1"/>
-        <v>7.3873946781731066</v>
+        <v>9.8062761214687271</v>
       </c>
       <c r="G4" s="10">
         <f t="shared" si="1"/>
-        <v>9.8498595708974754</v>
+        <v>13.075034828624968</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="45">
         <v>0.68432000000000004</v>
       </c>
       <c r="C5" s="10">
         <f t="shared" si="1"/>
-        <v>4.170816101452</v>
+        <v>5.5364815506000005</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" si="1"/>
-        <v>6.2562241521780004</v>
+        <v>8.3047223259000003</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" si="1"/>
-        <v>8.341632202904</v>
+        <v>11.072963101200001</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" si="1"/>
-        <v>12.512448304356001</v>
+        <v>16.609444651800001</v>
       </c>
       <c r="G5" s="10">
         <f t="shared" si="1"/>
-        <v>16.683264405808</v>
+        <v>22.145926202400002</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="36">
         <v>0.96462000000000003</v>
       </c>
       <c r="C6" s="10">
         <f t="shared" si="1"/>
-        <v>5.8791977843445</v>
+        <v>7.8042448464750001</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="1"/>
-        <v>8.8187966765167509</v>
+        <v>11.7063672697125</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="1"/>
-        <v>11.758395568689</v>
+        <v>15.60848969295</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>17.637593353033502</v>
+        <v>23.412734539424999</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" si="1"/>
-        <v>23.516791137378</v>
+        <v>31.2169793859</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="37">
         <v>0.86746324999999902</v>
       </c>
       <c r="C7" s="14">
         <f>$B7*($B$11-$B$10)*$B$12*(C$2/1000)</f>
-        <v>5.2870436207006621</v>
+        <v>7.0181994965053045</v>
       </c>
       <c r="D7" s="14">
         <f>$B7*($B$11-$B$10)*$B$12*(D$2/1000)</f>
-        <v>7.9305654310509937</v>
+        <v>10.527299244757957</v>
       </c>
       <c r="E7" s="14">
         <f>$B7*($B$11-$B$10)*$B$12*(E$2/1000)</f>
-        <v>10.574087241401324</v>
+        <v>14.036398993010609</v>
       </c>
       <c r="F7" s="14">
         <f>$B7*($B$11-$B$10)*$B$12*(F$2/1000)</f>
-        <v>15.861130862101987</v>
+        <v>21.054598489515914</v>
       </c>
       <c r="G7" s="14">
         <f>$B7*($B$11-$B$10)*$B$12*(G$2/1000)</f>
-        <v>21.148174482802649</v>
+        <v>28.072797986021218</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -11230,7 +11235,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="19">
-        <v>2243</v>
+        <v>2650</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>38</v>
@@ -11250,6 +11255,13 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
+      <c r="F12">
+        <v>10.16</v>
+      </c>
+      <c r="G12" s="44">
+        <f>F12/((B11-B10)*B12*(59/1000))</f>
+        <v>1.0642338699389575E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -11257,6 +11269,10 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
+      <c r="G13">
+        <f>G12/B7</f>
+        <v>1.226834531536591E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
subplot of all modes of transport (bedload included)
</commit_message>
<xml_diff>
--- a/Shear Stress/bedload_tauc/Wilcock2002_tauc.xlsx
+++ b/Shear Stress/bedload_tauc/Wilcock2002_tauc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Shear Stress\bedload_tauc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E15671B-F4DD-4FD7-B4F8-A956E73685BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A66BE3-DD0B-48AC-BEE7-DB7CC6DD94A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
+    <workbookView xWindow="-12555" yWindow="330" windowWidth="12480" windowHeight="15150" activeTab="2" xr2:uid="{3E16E29A-D0FE-4C27-A7A7-0122C151A299}"/>
   </bookViews>
   <sheets>
     <sheet name="Dg-Ds Calculation" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Fs</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Dimensional Tauc by Size (mm) in Pa</t>
+  </si>
+  <si>
+    <t>Dimensional Tauc by Size (um) in Pa</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -458,6 +461,9 @@
     <xf numFmtId="165" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -474,6 +480,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7413,18 +7426,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="41"/>
+      <c r="C2" s="42"/>
       <c r="H2" s="18" t="s">
         <v>16</v>
       </c>
@@ -7723,12 +7736,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="24">
@@ -8163,10 +8176,10 @@
       <c r="F1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="44"/>
+      <c r="I1" s="45"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8195,11 +8208,11 @@
         <f>$I$20+($I$19-$I$20)*EXP(-14*A2)</f>
         <v>1.3290468742698638</v>
       </c>
-      <c r="H2" s="44" t="str">
+      <c r="H2" s="45" t="str">
         <f>B1</f>
         <v>Tri* (Dg/Ds = 10)</v>
       </c>
-      <c r="I2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8327,11 +8340,11 @@
         <f t="shared" si="4"/>
         <v>0.7870350317127095</v>
       </c>
-      <c r="H6" s="44" t="str">
+      <c r="H6" s="45" t="str">
         <f>C1</f>
         <v>Tri* (Dg/Ds = 20)</v>
       </c>
-      <c r="I6" s="44"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8459,11 +8472,11 @@
         <f t="shared" si="4"/>
         <v>0.4774329545306662</v>
       </c>
-      <c r="H10" s="44" t="str">
+      <c r="H10" s="45" t="str">
         <f>D1</f>
         <v>Tri* (Dg/Ds = 35)</v>
       </c>
-      <c r="I10" s="44"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -8591,11 +8604,11 @@
         <f t="shared" si="4"/>
         <v>0.30058544185786273</v>
       </c>
-      <c r="H14" s="44" t="str">
+      <c r="H14" s="45" t="str">
         <f>E1</f>
         <v>Tri* (Dg/Ds = 50)</v>
       </c>
-      <c r="I14" s="44"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -8720,11 +8733,11 @@
         <f t="shared" si="4"/>
         <v>0.1995685397000391</v>
       </c>
-      <c r="H18" s="44" t="str">
+      <c r="H18" s="45" t="str">
         <f>F1</f>
         <v>Tri* (Dg/Ds = 43.4)</v>
       </c>
-      <c r="I18" s="44"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -11002,10 +11015,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE20B856-AC4B-4A0B-8068-FF571A1CD20B}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11021,26 +11034,28 @@
     <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
@@ -11063,7 +11078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
@@ -11091,7 +11106,7 @@
         <v>7.0277199761999993</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
@@ -11119,7 +11134,7 @@
         <v>13.075034828624968</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
@@ -11147,7 +11162,7 @@
         <v>22.145926202400002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
@@ -11175,7 +11190,7 @@
         <v>31.2169793859</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>33</v>
       </c>
@@ -11203,21 +11218,21 @@
         <v>28.072797986021218</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -11230,7 +11245,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -11243,7 +11258,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -11263,7 +11278,7 @@
         <v>1.0642338699389575E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -11274,117 +11289,196 @@
         <v>1.226834531536591E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="48">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <f>$B$7*($B$11-$B$10)*$B$12*($A18/1000000)</f>
+        <v>2.8072797986021216E-2</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="48">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <f>$B$7*($B$11-$B$10)*$B$12*($A19/1000000)</f>
+        <v>0.2807279798602122</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="48">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" ref="B19:B29" si="2">$B$7*($B$11-$B$10)*$B$12*($A20/1000000)</f>
+        <v>0.63163795468547745</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="48">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.88429313655966835</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="49">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="2"/>
+        <v>1.403639899301061</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="49">
+        <v>200</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8072797986021221</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="49">
+        <v>280</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="2"/>
+        <v>3.9301917180429702</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="49">
+        <v>500</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="2"/>
+        <v>7.0181994965053045</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="49">
+        <v>700</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="2"/>
+        <v>9.8254792951074261</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="49">
+        <v>850</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="2"/>
+        <v>11.930939144059018</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="49">
+        <v>1000</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="2"/>
+        <v>14.036398993010609</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="40">
+        <v>1500</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="2"/>
+        <v>21.054598489515914</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="49">
+        <v>2000</v>
+      </c>
+      <c r="B30" s="2">
+        <f>$B$7*($B$11-$B$10)*$B$12*($A30/1000000)</f>
+        <v>28.072797986021218</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>

</xml_diff>